<commit_message>
Finished working on requirements section.
</commit_message>
<xml_diff>
--- a/data/processed/Keep Your Distance - Non Contact Evaluation.xlsx
+++ b/data/processed/Keep Your Distance - Non Contact Evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Ryan\Documents\University\4th_Year\Level_4_Project\Keep-Your-Distance\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF29CBC-8322-4377-ABDF-63CA6D25EE71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4211A534-CFC6-4632-8E38-D576ED287286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8850" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
+    <workbookView xWindow="-28920" yWindow="2925" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Eval" sheetId="2" r:id="rId1"/>
@@ -3011,9 +3011,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0099CC"/>
+      <color rgb="FFFF5050"/>
       <color rgb="FF00CC00"/>
-      <color rgb="FFFF5050"/>
-      <color rgb="FF0099CC"/>
       <color rgb="FFFF6699"/>
       <color rgb="FFFF9999"/>
       <color rgb="FF66FF66"/>
@@ -6946,8 +6946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9391,7 +9391,7 @@
   <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10165,7 +10165,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10207,13 +10207,13 @@
       <c r="K1" t="s">
         <v>721</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="14" t="s">
         <v>735</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="15" t="s">
         <v>736</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="16" t="s">
         <v>737</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Wrote Against system use section
</commit_message>
<xml_diff>
--- a/data/processed/Keep Your Distance - Non Contact Evaluation.xlsx
+++ b/data/processed/Keep Your Distance - Non Contact Evaluation.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Ryan\Documents\University\4th_Year\Level_4_Project\Keep-Your-Distance\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78D0FF4-096D-4145-A1D9-97F780B81E2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC1E51D-0180-4EF6-9706-BECD019ADF00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2925" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
+    <workbookView xWindow="-28920" yWindow="2925" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Eval" sheetId="2" r:id="rId1"/>
     <sheet name="Open Coding" sheetId="3" r:id="rId2"/>
-    <sheet name="Codes" sheetId="4" r:id="rId3"/>
-    <sheet name="Full Coding" sheetId="5" r:id="rId4"/>
+    <sheet name="Open Code Analysis Help" sheetId="6" r:id="rId3"/>
+    <sheet name="Codes" sheetId="4" r:id="rId4"/>
+    <sheet name="Full Coding" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="770">
   <si>
     <t>Would you consider yourself tech-literate (i.e. comfortable using technology and understanding technical terms such as IP address)?</t>
   </si>
@@ -1963,9 +1964,6 @@
     <t>Understood device number decrease</t>
   </si>
   <si>
-    <t>Misunderstood device number increase - thought safety</t>
-  </si>
-  <si>
     <t>O49</t>
   </si>
   <si>
@@ -2369,6 +2367,18 @@
   </si>
   <si>
     <t>Participant 24</t>
+  </si>
+  <si>
+    <t>Open Codes</t>
+  </si>
+  <si>
+    <t>Misunderstood device number decrease - thought safety</t>
+  </si>
+  <si>
+    <t>Tech-Literate</t>
+  </si>
+  <si>
+    <t>Totals</t>
   </si>
 </sst>
 </file>
@@ -2782,7 +2792,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2897,6 +2907,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2942,7 +2967,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2962,6 +2987,9 @@
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6946,7 +6974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
@@ -7443,19 +7471,19 @@
         <v>550</v>
       </c>
       <c r="J9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="K9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="Q9" t="s">
         <v>586</v>
       </c>
       <c r="T9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="V9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -7640,10 +7668,10 @@
         <v>603</v>
       </c>
       <c r="C16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E16" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F16" t="s">
         <v>587</v>
@@ -7804,13 +7832,13 @@
         <v>555</v>
       </c>
       <c r="J20" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="K20" t="s">
         <v>583</v>
       </c>
       <c r="Q20" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -8162,13 +8190,13 @@
         <v>562</v>
       </c>
       <c r="C28" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G28" t="s">
         <v>551</v>
@@ -8177,13 +8205,13 @@
         <v>551</v>
       </c>
       <c r="R28" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="X28" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="Y28" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
@@ -8339,22 +8367,22 @@
         <v>563</v>
       </c>
       <c r="C34" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E34" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F34" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G34" t="s">
         <v>563</v>
       </c>
       <c r="J34" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="K34" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
@@ -8710,11 +8738,11 @@
       </c>
       <c r="B42" s="3"/>
       <c r="C42" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
@@ -8731,7 +8759,7 @@
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
       <c r="R42" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
@@ -8797,7 +8825,7 @@
         <v>571</v>
       </c>
       <c r="S43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="T43" t="s">
         <v>571</v>
@@ -8874,7 +8902,7 @@
         <v>574</v>
       </c>
       <c r="S44" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="T44" t="s">
         <v>574</v>
@@ -8903,34 +8931,34 @@
         <v>577</v>
       </c>
       <c r="C45" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D45" t="s">
         <v>576</v>
       </c>
       <c r="E45" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F45" t="s">
         <v>576</v>
       </c>
       <c r="G45" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="H45" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I45" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="J45" t="s">
         <v>576</v>
       </c>
       <c r="K45" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="L45" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="M45" t="s">
         <v>576</v>
@@ -8939,10 +8967,10 @@
         <v>577</v>
       </c>
       <c r="O45" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="P45" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="Q45" t="s">
         <v>576</v>
@@ -8954,22 +8982,22 @@
         <v>577</v>
       </c>
       <c r="T45" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="U45" t="s">
         <v>577</v>
       </c>
       <c r="V45" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="W45" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="X45" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="Y45" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
@@ -9057,73 +9085,73 @@
         <v>582</v>
       </c>
       <c r="C47" t="s">
+        <v>644</v>
+      </c>
+      <c r="D47" t="s">
         <v>645</v>
       </c>
-      <c r="D47" t="s">
-        <v>646</v>
-      </c>
       <c r="E47" t="s">
+        <v>644</v>
+      </c>
+      <c r="F47" t="s">
         <v>645</v>
       </c>
-      <c r="F47" t="s">
-        <v>646</v>
-      </c>
       <c r="G47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="H47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="K47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="L47" t="s">
+        <v>644</v>
+      </c>
+      <c r="M47" t="s">
         <v>645</v>
       </c>
-      <c r="M47" t="s">
-        <v>646</v>
-      </c>
       <c r="N47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="O47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="P47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="Q47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="R47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="S47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="T47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="U47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="V47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="W47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="X47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="Y47" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
@@ -9163,28 +9191,28 @@
         <v>583</v>
       </c>
       <c r="C49" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D49" t="s">
         <v>584</v>
       </c>
       <c r="E49" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H49" t="s">
         <v>583</v>
       </c>
       <c r="I49" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J49" t="s">
         <v>583</v>
       </c>
       <c r="K49" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="M49" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="N49" t="s">
         <v>583</v>
@@ -9193,7 +9221,7 @@
         <v>584</v>
       </c>
       <c r="Q49" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="S49" t="s">
         <v>583</v>
@@ -9205,7 +9233,7 @@
         <v>584</v>
       </c>
       <c r="V49" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="W49" t="s">
         <v>584</v>
@@ -9225,16 +9253,16 @@
         <v>584</v>
       </c>
       <c r="C50" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D50" t="s">
         <v>585</v>
       </c>
       <c r="E50" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G50" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="H50" t="s">
         <v>585</v>
@@ -9243,25 +9271,25 @@
         <v>585</v>
       </c>
       <c r="L50" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="M50" t="s">
         <v>585</v>
       </c>
       <c r="N50" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="O50" t="s">
         <v>585</v>
       </c>
       <c r="P50" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="R50" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="S50" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="T50" t="s">
         <v>585</v>
@@ -9387,11 +9415,1137 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1331F00-DFC4-4A87-ABBB-99ABB069364E}">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="98.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B1" t="s">
+        <v>766</v>
+      </c>
+      <c r="C1" t="s">
+        <v>768</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>577</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>634</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>579</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>580</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>582</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>644</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="K1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>742</v>
+      </c>
+      <c r="B2" t="str" cm="1">
+        <f t="array" ref="B2:B25">TRANSPOSE('Open Coding'!B51:Y51)</f>
+        <v>O1,O4,O7,Q10,O12,O13,O14,O15,O17,O18,O20,O22,O24,O25,O26,O28,O30,O33,O34,O37,O40,O42,O43,O44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="18">
+        <f>IF(ISNUMBER(SEARCH(D$1,$B2)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B2)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B2)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B2)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B2)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="17">
+        <f t="shared" ref="E2:K17" si="0">IF(ISNUMBER(SEARCH(I$1,$B2)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f>SUM(D2:J2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>743</v>
+      </c>
+      <c r="B3" t="str">
+        <v>O1,O4,O8,O9,O46,O13,O47,O15,O48,O18,O20,O22,O49,O50,O26,O29,O30,O51,O33,O34,O53,O38,O54,O56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="18">
+        <f t="shared" ref="D3:K25" si="1">IF(ISNUMBER(SEARCH(D$1,$B3)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B3)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B3)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B3)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B3)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J3" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K25" si="2">SUM(D3:J3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>744</v>
+      </c>
+      <c r="B4" t="str">
+        <v>O2,O4,O7,O10,O15,O18,O20,O22,O26,O28,O30,O33,O34,O36,O38,O55,O44,O45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B4)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B4)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B4)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B4)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>745</v>
+      </c>
+      <c r="B5" t="str">
+        <v>O2,O5,O8,O9,O57,O16,O17,O18,O20,O22,O58,O59,O26,O28,O30,O33,O34,O53,O38,O54,O56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B5)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B5)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B5)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B5)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>746</v>
+      </c>
+      <c r="B6" t="str">
+        <v>O2,O4,O7,O9,O47,O15,O18,O20,O22,O49,O58,O50,O26,O28,O30,O33,O34,O36,O38,O55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B6)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B6)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B6)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B6)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>747</v>
+      </c>
+      <c r="B7" t="str">
+        <v>O1,O4,O7,O11,O12,O15,O18,O20,O22,O13,O25,O26,O28,O30,O31,O32,O34,O52,O40,O55,O60,O61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B7)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B7)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B7)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B7)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>748</v>
+      </c>
+      <c r="B8" t="str">
+        <v>O1,O4,O7,O10,O15,O18,O20,O22,O26,O28,O30,O33,O34,O52,O38,O55,O43,O45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B8)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B8)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B8)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B8)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>749</v>
+      </c>
+      <c r="B9" t="str">
+        <v>O2,O5,O8,O9,O16,O18,O20,O22,O26,O28,O31,O32,O34,O53,O40,O55,O62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B9)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B9)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B9)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H9" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B9)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>750</v>
+      </c>
+      <c r="B10" t="str">
+        <v>O1,O4,O7,O9,O63,O16,O64,O18,O20,O22,O13,O26,O28,O31,O32,O34,O36,O38,O55,O43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B10)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B10)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B10)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B10)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>751</v>
+      </c>
+      <c r="B11" t="str">
+        <v>O1,O4,O7,O9,O65,O47,O15,O43,O18,O20,O22,O50,O66,O26,O28,O30,O33,O34,O53,O40,O55,O62,O45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B11)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B11)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B11)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B11)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>752</v>
+      </c>
+      <c r="B12" t="str">
+        <v>O1,O5,O8,O9,O15,O18,O20,O22,O26,O28,O30,O33,O34,O52,O38,O54,O67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B12)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B12)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B12)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B12)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J12" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>753</v>
+      </c>
+      <c r="B13" t="str">
+        <v>O1,O5,O8,O9,O15,O19,O20,O22,O26,O28,O30,O32,O34,O36,O38,O55,O62,O68,O45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B13)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B13)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B13)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B13)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>754</v>
+      </c>
+      <c r="B14" t="str">
+        <v>O1,O4,O7,O9,O16,O20,O22,O26,O28,O30,O33,O34,O37,O39,O55,O43,O56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B14)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B14)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B14)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B14)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>755</v>
+      </c>
+      <c r="B15" t="str">
+        <v>O1,O4,O7,O9,O15,O18,O20,O22,O26,O28,O30,O33,O34,O52,O39,O55,O44,O45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B15)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B15)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B15)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B15)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>756</v>
+      </c>
+      <c r="B16" t="str">
+        <v>O2,O5,O8,O10,O15,O18,O20,O22,O26,O28,O30,O32,O34,O53,O38,O55,O59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B16)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B16)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B16)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B16)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>757</v>
+      </c>
+      <c r="B17" t="str">
+        <v>O1,O4,O7,O9,O46,O16,O69,O19,O20,O22,O26,O29,O30,O33,O34,O36,O38,O55,O65</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B17)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B17)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B17)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B17)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>758</v>
+      </c>
+      <c r="B18" t="str">
+        <v>O2,O5,O7,O10,O16,O18,O20,O22,O70,O26,O28,O31,O71,O33,O34,O36,O40,O55,O72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B18)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B18)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B18)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H18" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B18)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>759</v>
+      </c>
+      <c r="B19" t="str">
+        <v>O2,O4,O7,O9,O15,O19,O20,O22,O26,O28,O30,O73,O74,O37,O39,O55,O43,O67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B19)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B19)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B19)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B19)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>760</v>
+      </c>
+      <c r="B20" t="str">
+        <v>O2,O5,O8,O9,O65,O15,O18,O20,O22,O26,O28,O30,O33,O34,O53,O40,O55,O44,O45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B20)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B20)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B20)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H20" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B20)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>761</v>
+      </c>
+      <c r="B21" t="str">
+        <v>O2,O4,O7,O11,O16,O20,O22,O26,O29,O31,O33,O34,O37,O39,O55,O44,O45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B21)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B21)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B21)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B21)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>762</v>
+      </c>
+      <c r="B22" t="str">
+        <v>O1,O4,O7,O11,O65,O15,O18,O20,O22,O26,O28,O31,O33,O34,O53,O38,O55,O75,O43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B22)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B22)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B22)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B22)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>763</v>
+      </c>
+      <c r="B23" t="str">
+        <v>O1,O5,O8,O10,O16,O19,O20,O23,O27,O29,O31,O33,O34,O52,O39,O55,O44,O45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B23)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B23)),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G23" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B23)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B23)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>764</v>
+      </c>
+      <c r="B24" t="str">
+        <v>O2,O5,O8,O9,O47,O15,O18,O20,O22,O76,O26,O28,O30,O33,O34,O53,O38,O55,O44,O45</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B24)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B24)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B24)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B24)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>765</v>
+      </c>
+      <c r="B25" t="str">
+        <v>O1,O5,O8,O9,O15,O18,O20,O22,O76,O26,O28,O30,O32,O34,O53,O38,O54,O44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="18">
+        <f>IF(ISNUMBER(SEARCH(E$1,$B25)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="19">
+        <f>IF(ISNUMBER(SEARCH(F$1,$B25)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="19">
+        <f>IF(ISNUMBER(SEARCH(G$1,$B25)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="17">
+        <f>IF(ISNUMBER(SEARCH(H$1,$B25)),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J25" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>769</v>
+      </c>
+      <c r="D26" s="18">
+        <f>SUM(D2:D25)</f>
+        <v>4</v>
+      </c>
+      <c r="E26" s="18">
+        <f>SUM(E2:E25)</f>
+        <v>5</v>
+      </c>
+      <c r="F26" s="19">
+        <f>SUM(F2:F25)</f>
+        <v>5</v>
+      </c>
+      <c r="G26" s="19">
+        <f>SUM(G2:G25)</f>
+        <v>6</v>
+      </c>
+      <c r="H26" s="17">
+        <f>SUM(H2:H25)</f>
+        <v>1</v>
+      </c>
+      <c r="I26" s="17">
+        <f t="shared" ref="E26:J26" si="3">SUM(I2:I25)</f>
+        <v>4</v>
+      </c>
+      <c r="J26" s="17">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="K26">
+        <f>SUM(K2:K25)</f>
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9411,13 +10565,13 @@
         <v>539</v>
       </c>
       <c r="D1" t="s">
+        <v>698</v>
+      </c>
+      <c r="E1" t="s">
         <v>699</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>700</v>
-      </c>
-      <c r="F1" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -9428,13 +10582,13 @@
         <v>572</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9445,13 +10599,13 @@
         <v>573</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="F3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9462,13 +10616,13 @@
         <v>589</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="F4" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -9479,13 +10633,13 @@
         <v>593</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F5" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -9496,10 +10650,10 @@
         <v>594</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="F6" t="s">
         <v>540</v>
@@ -9513,13 +10667,13 @@
         <v>590</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F7" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -9530,13 +10684,13 @@
         <v>591</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F8" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -9547,13 +10701,13 @@
         <v>592</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F9" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -9564,13 +10718,13 @@
         <v>596</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F10" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -9581,13 +10735,13 @@
         <v>597</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F11" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -9606,13 +10760,13 @@
         <v>600</v>
       </c>
       <c r="D13" t="s">
+        <v>730</v>
+      </c>
+      <c r="E13" t="s">
         <v>731</v>
       </c>
-      <c r="E13" t="s">
-        <v>732</v>
-      </c>
       <c r="F13" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9623,13 +10777,13 @@
         <v>601</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9640,13 +10794,13 @@
         <v>602</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -9657,13 +10811,13 @@
         <v>604</v>
       </c>
       <c r="D16" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>738</v>
-      </c>
       <c r="F16" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -9879,7 +11033,7 @@
         <v>582</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>631</v>
+        <v>767</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -9887,7 +11041,7 @@
         <v>583</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -9895,7 +11049,7 @@
         <v>584</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -9903,7 +11057,7 @@
         <v>585</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -9911,7 +11065,7 @@
         <v>586</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -9919,7 +11073,7 @@
         <v>587</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -9927,231 +11081,231 @@
         <v>588</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
   </sheetData>
@@ -10160,7 +11314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8924D6-3533-4AFC-98C2-1287BC453D4C}">
   <dimension ref="A1:N26"/>
   <sheetViews>
@@ -10175,51 +11329,51 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B1" t="s">
+        <v>701</v>
+      </c>
+      <c r="C1" t="s">
         <v>702</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>703</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>704</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>705</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>706</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>707</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>708</v>
       </c>
-      <c r="I1" t="s">
-        <v>709</v>
-      </c>
       <c r="J1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="K1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="L1" s="14" t="s">
+        <v>734</v>
+      </c>
+      <c r="M1" s="15" t="s">
         <v>735</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="16" t="s">
         <v>736</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B2">
         <v>7</v>
@@ -10266,7 +11420,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -10313,7 +11467,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -10360,7 +11514,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -10407,7 +11561,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B6">
         <v>8</v>
@@ -10454,7 +11608,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -10501,7 +11655,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -10548,7 +11702,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -10595,7 +11749,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -10642,7 +11796,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -10689,7 +11843,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B12">
         <v>8</v>
@@ -10736,7 +11890,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B13">
         <v>7</v>
@@ -10783,7 +11937,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -10830,7 +11984,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B15">
         <v>8</v>
@@ -10877,7 +12031,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B16">
         <v>7</v>
@@ -10924,7 +12078,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -10971,7 +12125,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -11018,7 +12172,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B19">
         <v>7</v>
@@ -11065,7 +12219,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -11112,7 +12266,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -11159,7 +12313,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -11206,7 +12360,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -11253,7 +12407,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B24">
         <v>8</v>
@@ -11300,7 +12454,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B25">
         <v>8</v>

</xml_diff>